<commit_message>
Commoi and push By Abhishek K- LoginPage
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15720" windowHeight="6540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Opportunities" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:L20"/>
 </workbook>
 </file>
 
@@ -780,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -933,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
commit and push by Abhishek k- TC_15
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15720" windowHeight="6540" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="1" r:id="rId1"/>
     <sheet name="Contacts" sheetId="2" r:id="rId2"/>
     <sheet name="Products" sheetId="3" r:id="rId3"/>
     <sheet name="MultipleOrg" sheetId="4" r:id="rId4"/>
-    <sheet name="Vendor" sheetId="5" r:id="rId5"/>
+    <sheet name="Vendors" sheetId="5" r:id="rId5"/>
     <sheet name="Opportunities" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:L20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>TC_ID</t>
   </si>
@@ -46,9 +45,6 @@
     <t>Industry_Name</t>
   </si>
   <si>
-    <t>Qspiders</t>
-  </si>
-  <si>
     <t>TC_03</t>
   </si>
   <si>
@@ -79,15 +75,9 @@
     <t>Vender_Name</t>
   </si>
   <si>
-    <t>Abhishek</t>
-  </si>
-  <si>
     <t>Product_Name</t>
   </si>
   <si>
-    <t>Oneplus</t>
-  </si>
-  <si>
     <t>Industry_Type</t>
   </si>
   <si>
@@ -212,6 +202,21 @@
   </si>
   <si>
     <t>Samgsung s25</t>
+  </si>
+  <si>
+    <t>IAmFromBidar</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>Vendors_Name</t>
+  </si>
+  <si>
+    <t>Oneplus_11r</t>
+  </si>
+  <si>
+    <t>Abhishek Kelusker</t>
   </si>
 </sst>
 </file>
@@ -593,7 +598,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -622,7 +627,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -641,16 +646,16 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -694,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -705,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -714,33 +719,33 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -752,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>2</v>
@@ -760,16 +765,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -781,14 +786,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -800,24 +805,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -828,18 +833,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -866,63 +871,63 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -932,10 +937,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -953,18 +958,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -975,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
@@ -983,16 +988,35 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1026,42 +1050,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>